<commit_message>
a huge update adding check in , check out with total time display
</commit_message>
<xml_diff>
--- a/uploads/excelData.xlsx
+++ b/uploads/excelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce5ca035ce437d53/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4B96BEB-854C-42F0-896F-D348CD4F716E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{E4B96BEB-854C-42F0-896F-D348CD4F716E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5114667F-4572-400F-9ECF-4F5806042C6F}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{4848C951-CB1B-4DA9-B3A5-75413F38B98D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4848C951-CB1B-4DA9-B3A5-75413F38B98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>fullname</t>
   </si>
@@ -42,34 +42,61 @@
     <t>email</t>
   </si>
   <si>
+    <t>classs</t>
+  </si>
+  <si>
+    <t>AHETESHAM URRAB</t>
+  </si>
+  <si>
+    <t>ahete@gmail.com</t>
+  </si>
+  <si>
+    <t>TYBBACA</t>
+  </si>
+  <si>
+    <t>alid@gmail.com</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>FIRDOUS</t>
+  </si>
+  <si>
+    <t>ALID SHAUKH</t>
+  </si>
+  <si>
+    <t>sid</t>
+  </si>
+  <si>
     <t>roll</t>
   </si>
   <si>
-    <t>classs</t>
-  </si>
-  <si>
-    <t>qrCode</t>
-  </si>
-  <si>
-    <t>AHETESHAM URRAB</t>
-  </si>
-  <si>
-    <t>ahete@gmail.com</t>
-  </si>
-  <si>
-    <t>TYBBACA</t>
-  </si>
-  <si>
-    <t>ALID SHAIKH</t>
-  </si>
-  <si>
-    <t>alid@gmail.com</t>
-  </si>
-  <si>
-    <t>SALAUDDIN SAYYED</t>
-  </si>
-  <si>
-    <t>salau@gmail.com</t>
+    <t>MOHAMMED MAAZ SHAIKH</t>
+  </si>
+  <si>
+    <t>SALAUDDIN KHAN</t>
+  </si>
+  <si>
+    <t>ABUSHAMA</t>
+  </si>
+  <si>
+    <t>maaz@gmail.com</t>
+  </si>
+  <si>
+    <t>firdous@gmail.com</t>
+  </si>
+  <si>
+    <t>salaudin@gmail.com</t>
+  </si>
+  <si>
+    <t>abu@gmail.com</t>
+  </si>
+  <si>
+    <t>UZMA SAYYED</t>
+  </si>
+  <si>
+    <t>uzma@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -114,9 +141,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -133,6 +163,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,21 +466,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF18829-CAC1-4775-BF76-4703EA51A6E6}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,64 +489,135 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2">
+        <v>3803556</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+      <c r="E2">
         <v>6623</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>2355786222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>4087370</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>6656</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>6670</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>3468992277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4">
+        <v>3800563</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>6674</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>3801330</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>6675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>3801322</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>6617</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>6826356342</v>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>3801332</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>6640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>3803389</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>6626</v>
       </c>
     </row>
   </sheetData>
@@ -519,6 +625,10 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{88B0CE95-2004-4221-9BA2-AE345354343E}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{E10D0610-F4A1-4EBE-B405-500E3C843B7B}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{EC573C02-6AC3-49B0-B9D5-8ED254D96832}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{30B19D47-8013-47FA-90FC-E73C9B60982E}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{8DEFCEAE-48AB-480D-9323-1284B679E7D8}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{65E23494-53AC-46F3-9AC9-CA30B6776F6F}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{519C2571-4704-4A35-9E27-33EAAEC685B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adds the batch module
</commit_message>
<xml_diff>
--- a/uploads/excelData.xlsx
+++ b/uploads/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce5ca035ce437d53/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{E4B96BEB-854C-42F0-896F-D348CD4F716E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5114667F-4572-400F-9ECF-4F5806042C6F}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{E4B96BEB-854C-42F0-896F-D348CD4F716E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBA46655-0DB9-437D-BA2B-9F6AF65E0489}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4848C951-CB1B-4DA9-B3A5-75413F38B98D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>fullname</t>
   </si>
@@ -97,6 +97,144 @@
   </si>
   <si>
     <t>uzma@gmail.com</t>
+  </si>
+  <si>
+    <t>hussain@gmail.com</t>
+  </si>
+  <si>
+    <t>HUSSAIN SAYYED</t>
+  </si>
+  <si>
+    <t>MUSAB DESHMUKH</t>
+  </si>
+  <si>
+    <t>musab@gmail.com</t>
+  </si>
+  <si>
+    <t>SAQIB BASHIR DUSTE</t>
+  </si>
+  <si>
+    <t>saquib@gmail.com</t>
+  </si>
+  <si>
+    <t>AMAAN MAINODDIN SHAIKH</t>
+  </si>
+  <si>
+    <t>amman@gmail.com</t>
+  </si>
+  <si>
+    <t>HAARIS AHMED MATEEN SHAIKH</t>
+  </si>
+  <si>
+    <t>ZIDAAN AASIF TAMBOLI</t>
+  </si>
+  <si>
+    <t>ASAD MOULALI SHAIKH</t>
+  </si>
+  <si>
+    <t>ADITYA PRAKASH SONULE</t>
+  </si>
+  <si>
+    <t>MUSKAN IRFAN PATWEKAR</t>
+  </si>
+  <si>
+    <t>ARYAN SACHIN GAIKWAD</t>
+  </si>
+  <si>
+    <t>AKIL SHAKIL FARAS</t>
+  </si>
+  <si>
+    <t>MD JUNAID ASHRAF SHAIKH</t>
+  </si>
+  <si>
+    <t>UDAY RAJESH SHINDE</t>
+  </si>
+  <si>
+    <t>HUSSAIN ABBAS SAYYED</t>
+  </si>
+  <si>
+    <t>RUHANA SARFRAZ JAHAGIRDAR</t>
+  </si>
+  <si>
+    <t>DEVENDRA HANUMANTH GAIKWAD</t>
+  </si>
+  <si>
+    <t>SAHIL ALI MUSHTAQUE ALI SHAIKH</t>
+  </si>
+  <si>
+    <t>SHOAIB SAMEER SHAIKH</t>
+  </si>
+  <si>
+    <t>ALTAF NABI KAKANDKI</t>
+  </si>
+  <si>
+    <t>MOHAMMED NATIQ HASAN SAYYED</t>
+  </si>
+  <si>
+    <t>TAAHA KHALID SIDDIQUI</t>
+  </si>
+  <si>
+    <t>RASAAM NAEEM BHALDAR</t>
+  </si>
+  <si>
+    <t>MUFIZ QUTBUDDIN SHAIKH</t>
+  </si>
+  <si>
+    <t>haaris@gmail.com</t>
+  </si>
+  <si>
+    <t>zidan@gmail.com</t>
+  </si>
+  <si>
+    <t>naruto@gmail.com</t>
+  </si>
+  <si>
+    <t>ceo@gmail.com</t>
+  </si>
+  <si>
+    <t>ncc@gmail.com</t>
+  </si>
+  <si>
+    <t>ayan@gmail.com</t>
+  </si>
+  <si>
+    <t>akil@gamil.com</t>
+  </si>
+  <si>
+    <t>junu@gamil.com</t>
+  </si>
+  <si>
+    <t>uday@gamil.com</t>
+  </si>
+  <si>
+    <t>husssain@gamil.com</t>
+  </si>
+  <si>
+    <t>ruhana@gamil.com</t>
+  </si>
+  <si>
+    <t>dev@gamil.com</t>
+  </si>
+  <si>
+    <t>sahil@gamil.com</t>
+  </si>
+  <si>
+    <t>sammer@gamil.com</t>
+  </si>
+  <si>
+    <t>altaf@gamil.com</t>
+  </si>
+  <si>
+    <t>natiq@gamil.com</t>
+  </si>
+  <si>
+    <t>taha@gamil.com</t>
+  </si>
+  <si>
+    <t>rassam@gamil.com</t>
+  </si>
+  <si>
+    <t>mufiz@gamil.com</t>
   </si>
 </sst>
 </file>
@@ -466,16 +604,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF18829-CAC1-4775-BF76-4703EA51A6E6}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
@@ -618,6 +756,397 @@
       </c>
       <c r="E8">
         <v>6626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>3803554</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>6618</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>3801801</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>6605</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>3803349</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>6602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>3800982</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>6607</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>3848678</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>6609</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>3995727</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>6610</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>4813594</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>6613</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>3800943</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>6625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>3802610</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>6624</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18">
+        <v>3801327</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>6651</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19">
+        <v>3997262</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>6655</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20">
+        <v>3801331</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21">
+        <v>4261020</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>6679</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22">
+        <v>3998954</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>6677</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23">
+        <v>3848309</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>6676</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <v>4002311</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>6663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>3803431</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>6661</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26">
+        <v>3801362</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>6653</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27">
+        <v>3848745</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>6648</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28">
+        <v>3803350</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>6638</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29">
+        <v>4012808</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>6635</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30">
+        <v>3800825</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>6634</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31">
+        <v>4851066</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>6628</v>
       </c>
     </row>
   </sheetData>
@@ -629,6 +1158,29 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{8DEFCEAE-48AB-480D-9323-1284B679E7D8}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{65E23494-53AC-46F3-9AC9-CA30B6776F6F}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{519C2571-4704-4A35-9E27-33EAAEC685B6}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{018FE3B3-F41B-4274-80A5-57061CA1FDF2}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{B336EC3D-430C-4C84-AD08-405A5D17933E}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{26BD7E27-D819-408A-ACF2-A8DCFDDADA51}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{27E73E49-AF6F-4CA5-928E-1EC514E459BE}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{56F6EFFD-944C-4E75-9A57-8AEC9D4B5F97}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{F107EE24-669B-4964-90BB-9EC637C9149C}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{109D954A-8BF8-412C-8F01-515A6C4D7D5D}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{4FCA3E49-F227-472B-B99F-DDC36B520435}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{8DE4C606-27FE-4582-BD8E-E9E66135AA8B}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{09E467AB-8B43-4B83-B3B6-7559040E8414}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{24B2ADF0-F471-4F73-B35D-D27D649408B7}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{17EAE0F9-1102-4C3A-9C7A-037090D870B2}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{698594C2-5A19-42E0-8781-DE9D475EEA60}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{E50A1770-8397-49A9-9E7B-1B82E02D7BAF}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{BF73CA09-5CB5-4C3E-9BA2-D05C6702E5AA}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{300C8E6C-19A7-44FD-9602-0B6C6CF1E5E1}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{B126134E-2FF2-4686-8466-0CCD9BC36889}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{BE7F3683-F789-4AA8-B246-C5CC9D9CFEC2}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{9E8ED2FB-5714-41CF-9FEE-9F160B6B16B7}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{CCF634BC-E34B-4CA5-AD1B-2F7E8907999B}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{A63056B5-30E5-47A8-8F75-D9D826262D99}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{992AE992-9247-46B5-8331-99940C3367C0}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{A14D1969-5019-4D39-AA82-31DF96478C4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>